<commit_message>
Add objective functions interval charts
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="161"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="161" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="N = 100" sheetId="1" r:id="rId1"/>
+    <sheet name="Graphs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="25">
   <si>
     <t>Strategy</t>
   </si>
@@ -86,12 +87,24 @@
   <si>
     <t>Valido</t>
   </si>
+  <si>
+    <t>Mid</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -108,6 +121,11 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -129,7 +147,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -151,13 +169,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -168,6 +219,22 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -178,11 +245,1129 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Fuerza</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> de trabajo activa</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:stockChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$4:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>price_hours-0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>price_hours-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>price_hours-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>price_hours-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cost_price-0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>cost_price-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cost_price-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cost_price-6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$4:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>price_hours-0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>price_hours-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>price_hours-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>price_hours-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cost_price-0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>cost_price-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cost_price-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cost_price-6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$D$4:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.49938120167526</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.49358145940722</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.49818318298969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.49987121456185</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$4:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>price_hours-0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>price_hours-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>price_hours-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>price_hours-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cost_price-0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>cost_price-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cost_price-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cost_price-6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$E$4:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.99936533505155</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.9934168814433</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.99813659793814</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.99986791237113</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines/>
+        <c:axId val="-2146130888"/>
+        <c:axId val="-2144140472"/>
+      </c:stockChart>
+      <c:catAx>
+        <c:axId val="-2146130888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2144140472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2144140472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2146130888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ganancia</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:stockChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$12:$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>price_hours-0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>price_hours-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>price_hours-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>price_hours-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cost_price-0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>cost_price-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cost_price-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cost_price-6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$C$12:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7.719909724E7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.827016337E7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.888356824E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.938306893E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.545515329E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.460374429E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.416236624E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.446964964E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$12:$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>price_hours-0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>price_hours-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>price_hours-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>price_hours-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cost_price-0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>cost_price-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cost_price-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cost_price-6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$D$12:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7.343309724E7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.445216337E7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.503556824E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.551106893E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.177515329E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.096374429E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.054436624E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.083764964E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$12:$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>price_hours-0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>price_hours-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>price_hours-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>price_hours-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cost_price-0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>cost_price-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cost_price-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cost_price-6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$E$12:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7.531609724E7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.636116337E7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.695956824E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.744706893E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.361515329E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.278374429E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.235336624E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.265364964E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines/>
+        <c:axId val="2103840760"/>
+        <c:axId val="2103709752"/>
+      </c:stockChart>
+      <c:catAx>
+        <c:axId val="2103840760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2103709752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2103709752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2103840760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Costo de oportunidad</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:stockChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$20:$B$27</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>price_hours-0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>price_hours-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>price_hours-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>price_hours-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cost_price-0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>cost_price-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cost_price-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cost_price-6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$C$20:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.3132575548E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2976576439E8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3088968294E8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3101047756E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.34521349E8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3304300945E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3372319825E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3566332549E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$20:$B$27</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>price_hours-0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>price_hours-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>price_hours-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>price_hours-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cost_price-0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>cost_price-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cost_price-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cost_price-6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$D$20:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.2491975548E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2343576439E8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2450568294E8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2462047756E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.27959349E8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2655300945E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2719919825E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2904532549E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$20:$B$27</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>price_hours-0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>price_hours-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>price_hours-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>price_hours-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cost_price-0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>cost_price-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cost_price-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cost_price-6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$E$20:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.2812275548E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2660076439E8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2769768294E8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2781547756E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.31240349E8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2979800945E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3046119825E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3235432549E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines/>
+        <c:axId val="-2145520776"/>
+        <c:axId val="-2143195816"/>
+      </c:stockChart>
+      <c:catAx>
+        <c:axId val="-2145520776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2143195816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2143195816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2145520776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>132080</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>589280</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>147320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>284480</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>147320</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>5080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>5080</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -509,8 +1694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M801"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34:I36"/>
+    <sheetView topLeftCell="D3" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -12350,6 +13535,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
@@ -12362,4 +13548,673 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:I27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="8" max="9" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f>MIN(20,H4+I4)</f>
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <f>H4-I4</f>
+        <v>19.5</v>
+      </c>
+      <c r="E4">
+        <f>H4</f>
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <f>MIN(20,H5+I5)</f>
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <f>H5-I5</f>
+        <v>19.5</v>
+      </c>
+      <c r="E5">
+        <f>H5</f>
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <f>MIN(20,H6+I6)</f>
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <f>H6-I6</f>
+        <v>19.499381201675259</v>
+      </c>
+      <c r="E6">
+        <f>H6</f>
+        <v>19.999365335051547</v>
+      </c>
+      <c r="H6">
+        <v>19.999365335051547</v>
+      </c>
+      <c r="I6">
+        <v>0.49998413337628866</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <f>MIN(20,H7+I7)</f>
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <f>H7-I7</f>
+        <v>19.493581459407217</v>
+      </c>
+      <c r="E7">
+        <f>H7</f>
+        <v>19.993416881443299</v>
+      </c>
+      <c r="H7">
+        <v>19.993416881443299</v>
+      </c>
+      <c r="I7">
+        <v>0.4998354220360825</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <f>MIN(20,H8+I8)</f>
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <f>H8-I8</f>
+        <v>19.5</v>
+      </c>
+      <c r="E8">
+        <f>H8</f>
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <f>MIN(20,H9+I9)</f>
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <f>H9-I9</f>
+        <v>19.5</v>
+      </c>
+      <c r="E9">
+        <f>H9</f>
+        <v>20</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+      <c r="I9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <f>MIN(20,H10+I10)</f>
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <f>H10-I10</f>
+        <v>19.498183182989688</v>
+      </c>
+      <c r="E10">
+        <f>H10</f>
+        <v>19.998136597938142</v>
+      </c>
+      <c r="H10">
+        <v>19.998136597938142</v>
+      </c>
+      <c r="I10">
+        <v>0.49995341494845358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <f>MIN(20,H11+I11)</f>
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <f>H11-I11</f>
+        <v>19.499871214561853</v>
+      </c>
+      <c r="E11">
+        <f>H11</f>
+        <v>19.999867912371133</v>
+      </c>
+      <c r="H11">
+        <v>19.999867912371133</v>
+      </c>
+      <c r="I11">
+        <v>0.49999669780927836</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
+        <f>H12+I12</f>
+        <v>77199097.239999995</v>
+      </c>
+      <c r="D12" s="3">
+        <f>H12-I12</f>
+        <v>73433097.239999995</v>
+      </c>
+      <c r="E12" s="3">
+        <f>H12</f>
+        <v>75316097.239999995</v>
+      </c>
+      <c r="H12">
+        <v>75316097.239999995</v>
+      </c>
+      <c r="I12">
+        <v>1883000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3">
+        <f>H13+I13</f>
+        <v>78270163.370000005</v>
+      </c>
+      <c r="D13" s="3">
+        <f>H13-I13</f>
+        <v>74452163.370000005</v>
+      </c>
+      <c r="E13" s="3">
+        <f>H13</f>
+        <v>76361163.370000005</v>
+      </c>
+      <c r="H13">
+        <v>76361163.370000005</v>
+      </c>
+      <c r="I13">
+        <v>1909000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3">
+        <f>H14+I14</f>
+        <v>78883568.239999995</v>
+      </c>
+      <c r="D14" s="3">
+        <f>H14-I14</f>
+        <v>75035568.239999995</v>
+      </c>
+      <c r="E14" s="3">
+        <f>H14</f>
+        <v>76959568.239999995</v>
+      </c>
+      <c r="H14">
+        <v>76959568.239999995</v>
+      </c>
+      <c r="I14">
+        <v>1924000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3">
+        <f>H15+I15</f>
+        <v>79383068.930000007</v>
+      </c>
+      <c r="D15" s="3">
+        <f>H15-I15</f>
+        <v>75511068.930000007</v>
+      </c>
+      <c r="E15" s="3">
+        <f>H15</f>
+        <v>77447068.930000007</v>
+      </c>
+      <c r="H15">
+        <v>77447068.930000007</v>
+      </c>
+      <c r="I15">
+        <v>1936000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3">
+        <f>H16+I16</f>
+        <v>75455153.290000007</v>
+      </c>
+      <c r="D16" s="3">
+        <f>H16-I16</f>
+        <v>71775153.290000007</v>
+      </c>
+      <c r="E16" s="3">
+        <f>H16</f>
+        <v>73615153.290000007</v>
+      </c>
+      <c r="H16">
+        <v>73615153.290000007</v>
+      </c>
+      <c r="I16">
+        <v>1840000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="3">
+        <f>H17+I17</f>
+        <v>74603744.290000007</v>
+      </c>
+      <c r="D17" s="3">
+        <f>H17-I17</f>
+        <v>70963744.290000007</v>
+      </c>
+      <c r="E17" s="3">
+        <f>H17</f>
+        <v>72783744.290000007</v>
+      </c>
+      <c r="H17">
+        <v>72783744.290000007</v>
+      </c>
+      <c r="I17">
+        <v>1820000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3">
+        <f>H18+I18</f>
+        <v>74162366.239999995</v>
+      </c>
+      <c r="D18" s="3">
+        <f>H18-I18</f>
+        <v>70544366.239999995</v>
+      </c>
+      <c r="E18" s="3">
+        <f>H18</f>
+        <v>72353366.239999995</v>
+      </c>
+      <c r="H18">
+        <v>72353366.239999995</v>
+      </c>
+      <c r="I18">
+        <v>1809000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="3">
+        <f>H19+I19</f>
+        <v>74469649.640000001</v>
+      </c>
+      <c r="D19" s="3">
+        <f>H19-I19</f>
+        <v>70837649.640000001</v>
+      </c>
+      <c r="E19" s="3">
+        <f>H19</f>
+        <v>72653649.640000001</v>
+      </c>
+      <c r="H19">
+        <v>72653649.640000001</v>
+      </c>
+      <c r="I19">
+        <v>1816000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3">
+        <f>H20+I20</f>
+        <v>131325755.48</v>
+      </c>
+      <c r="D20" s="3">
+        <f>H20-I20</f>
+        <v>124919755.48</v>
+      </c>
+      <c r="E20" s="3">
+        <f>H20</f>
+        <v>128122755.48</v>
+      </c>
+      <c r="H20">
+        <v>128122755.48</v>
+      </c>
+      <c r="I20">
+        <v>3203000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3">
+        <f>H21+I21</f>
+        <v>129765764.39</v>
+      </c>
+      <c r="D21" s="3">
+        <f>H21-I21</f>
+        <v>123435764.39</v>
+      </c>
+      <c r="E21" s="3">
+        <f>H21</f>
+        <v>126600764.39</v>
+      </c>
+      <c r="H21">
+        <v>126600764.39</v>
+      </c>
+      <c r="I21">
+        <v>3165000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="3">
+        <f>H22+I22</f>
+        <v>130889682.94</v>
+      </c>
+      <c r="D22" s="3">
+        <f>H22-I22</f>
+        <v>124505682.94</v>
+      </c>
+      <c r="E22" s="3">
+        <f>H22</f>
+        <v>127697682.94</v>
+      </c>
+      <c r="H22">
+        <v>127697682.94</v>
+      </c>
+      <c r="I22">
+        <v>3192000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="3">
+        <f>H23+I23</f>
+        <v>131010477.56</v>
+      </c>
+      <c r="D23" s="3">
+        <f>H23-I23</f>
+        <v>124620477.56</v>
+      </c>
+      <c r="E23" s="3">
+        <f>H23</f>
+        <v>127815477.56</v>
+      </c>
+      <c r="H23">
+        <v>127815477.56</v>
+      </c>
+      <c r="I23">
+        <v>3195000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="3">
+        <f>H24+I24</f>
+        <v>134521349</v>
+      </c>
+      <c r="D24" s="3">
+        <f>H24-I24</f>
+        <v>127959349</v>
+      </c>
+      <c r="E24" s="3">
+        <f>H24</f>
+        <v>131240349</v>
+      </c>
+      <c r="H24">
+        <v>131240349</v>
+      </c>
+      <c r="I24">
+        <v>3281000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="3">
+        <f>H25+I25</f>
+        <v>133043009.45</v>
+      </c>
+      <c r="D25" s="3">
+        <f>H25-I25</f>
+        <v>126553009.45</v>
+      </c>
+      <c r="E25" s="3">
+        <f>H25</f>
+        <v>129798009.45</v>
+      </c>
+      <c r="H25">
+        <v>129798009.45</v>
+      </c>
+      <c r="I25">
+        <v>3245000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="3">
+        <f>H26+I26</f>
+        <v>133723198.25</v>
+      </c>
+      <c r="D26" s="3">
+        <f>H26-I26</f>
+        <v>127199198.25</v>
+      </c>
+      <c r="E26" s="3">
+        <f>H26</f>
+        <v>130461198.25</v>
+      </c>
+      <c r="H26">
+        <v>130461198.25</v>
+      </c>
+      <c r="I26">
+        <v>3262000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="3">
+        <f>H27+I27</f>
+        <v>135663325.49000001</v>
+      </c>
+      <c r="D27" s="3">
+        <f>H27-I27</f>
+        <v>129045325.48999999</v>
+      </c>
+      <c r="E27" s="3">
+        <f>H27</f>
+        <v>132354325.48999999</v>
+      </c>
+      <c r="H27">
+        <v>132354325.48999999</v>
+      </c>
+      <c r="I27">
+        <v>3309000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>